<commit_message>
RRTGM tuned and fit for SO analysis
</commit_message>
<xml_diff>
--- a/reduced_data/model_global_radiation_outputs_dt.xlsx
+++ b/reduced_data/model_global_radiation_outputs_dt.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13830" windowWidth="21600" xWindow="32400" yWindow="-2265"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="28680" yWindow="-4380"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -16,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,6 +31,12 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -53,12 +60,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -336,8 +349,8 @@
   </sheetPr>
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -428,47 +441,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CESM2-CAM6</t>
+          <t>GFDL-CM4</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.848867088659272</v>
+        <v>2.186757032981262</v>
       </c>
       <c r="C2" t="n">
-        <v>342.7084642350852</v>
+        <v>342.5877437170712</v>
       </c>
       <c r="D2" t="n">
-        <v>98.45515364622118</v>
+        <v>100.3937087020096</v>
       </c>
       <c r="E2" t="n">
-        <v>50.25975829148695</v>
+        <v>51.46774280566628</v>
       </c>
       <c r="F2" t="n">
-        <v>238.9454676892799</v>
+        <v>240.0076012722534</v>
       </c>
       <c r="G2" t="n">
-        <v>262.8657267267128</v>
+        <v>263.7915002727632</v>
       </c>
       <c r="H2" t="n">
-        <v>188.3477404629301</v>
+        <v>188.6080703896835</v>
       </c>
       <c r="I2" t="n">
-        <v>247.3416549354041</v>
+        <v>245.4032545100102</v>
       </c>
       <c r="J2" t="n">
-        <v>22.41880243176404</v>
+        <v>23.74107042416596</v>
       </c>
       <c r="K2" t="n">
-        <v>28.36311483888344</v>
+        <v>29.89123309083064</v>
       </c>
       <c r="L2" t="n">
-        <v>402.7929416845314</v>
+        <v>402.5350128074264</v>
       </c>
       <c r="M2" t="n">
-        <v>347.6421492145173</v>
+        <v>344.0836354766247</v>
       </c>
       <c r="N2" t="n">
-        <v>320.6662855434454</v>
+        <v>322.5632298647705</v>
       </c>
       <c r="O2">
         <f>D2-E2</f>
@@ -486,43 +499,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.534088097936574</v>
+        <v>2.186757032981262</v>
       </c>
       <c r="C3" t="n">
-        <v>342.779888457537</v>
+        <v>342.5877437170712</v>
       </c>
       <c r="D3" t="n">
-        <v>100.4083904175496</v>
+        <v>100.3937087020096</v>
       </c>
       <c r="E3" t="n">
-        <v>51.55012736302555</v>
+        <v>51.46774280566628</v>
       </c>
       <c r="F3" t="n">
-        <v>239.8377339332959</v>
+        <v>240.0076012722534</v>
       </c>
       <c r="G3" t="n">
-        <v>263.6420608064908</v>
+        <v>263.7915002727632</v>
       </c>
       <c r="H3" t="n">
-        <v>189.0064899718254</v>
+        <v>188.6080703896835</v>
       </c>
       <c r="I3" t="n">
-        <v>245.7023486477792</v>
+        <v>245.4032545100102</v>
       </c>
       <c r="J3" t="n">
-        <v>23.83945233849051</v>
+        <v>23.74107042416596</v>
       </c>
       <c r="K3" t="n">
-        <v>29.96499498055961</v>
+        <v>29.89123309083064</v>
       </c>
       <c r="L3" t="n">
-        <v>402.2199939620591</v>
+        <v>402.5350128074264</v>
       </c>
       <c r="M3" t="n">
-        <v>343.5805576357924</v>
+        <v>344.0836354766247</v>
       </c>
       <c r="N3" t="n">
-        <v>322.0981615462912</v>
+        <v>322.5632298647705</v>
       </c>
       <c r="O3">
         <f>D3-E3</f>
@@ -540,43 +553,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.885781777872787</v>
+        <v>3.691852852318956</v>
       </c>
       <c r="C4" t="n">
-        <v>339.4849955269531</v>
+        <v>339.2870044678376</v>
       </c>
       <c r="D4" t="n">
-        <v>103.7942326665021</v>
+        <v>103.6360544767424</v>
       </c>
       <c r="E4" t="n">
-        <v>46.34324205598809</v>
+        <v>46.22188581725988</v>
       </c>
       <c r="F4" t="n">
-        <v>232.8963557818814</v>
+        <v>233.0507340406619</v>
       </c>
       <c r="G4" t="n">
-        <v>262.1921213466793</v>
+        <v>262.3233375854765</v>
       </c>
       <c r="H4" t="n">
-        <v>178.3501115697088</v>
+        <v>178.2323115546925</v>
       </c>
       <c r="I4" t="n">
-        <v>245.0044576117705</v>
+        <v>244.8116497538489</v>
       </c>
       <c r="J4" t="n">
-        <v>16.35771583768421</v>
+        <v>16.30883527279584</v>
       </c>
       <c r="K4" t="n">
-        <v>22.83585544654365</v>
+        <v>22.76859991348907</v>
       </c>
       <c r="L4" t="n">
-        <v>402.8211876242225</v>
+        <v>403.1276070175356</v>
       </c>
       <c r="M4" t="n">
-        <v>345.3349394691361</v>
+        <v>345.6563692226257</v>
       </c>
       <c r="N4" t="n">
-        <v>319.3176880713557</v>
+        <v>319.733853562122</v>
       </c>
       <c r="O4">
         <f>D4-E4</f>
@@ -590,47 +603,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MRI-ESM2</t>
+          <t>IPSL-CM6A-LR</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.036277914891514</v>
+        <v>3.691160678863525</v>
       </c>
       <c r="C5" t="n">
-        <v>342.7713179570524</v>
+        <v>343.6947631835938</v>
       </c>
       <c r="D5" t="n">
-        <v>98.78611803032139</v>
+        <v>101.1413116455078</v>
       </c>
       <c r="E5" t="n">
-        <v>53.97546930750589</v>
+        <v>52.35886001586914</v>
       </c>
       <c r="F5" t="n">
-        <v>239.9489220118395</v>
+        <v>238.8623504638672</v>
       </c>
       <c r="G5" t="n">
-        <v>264.3077792811944</v>
+        <v>263.935791015625</v>
       </c>
       <c r="H5" t="n">
-        <v>192.4933452798664</v>
+        <v>189.9535064697266</v>
       </c>
       <c r="I5" t="n">
-        <v>245.8657745277478</v>
+        <v>249.1511383056641</v>
       </c>
       <c r="J5" t="n">
-        <v>26.85690586361529</v>
+        <v>23.22990036010742</v>
       </c>
       <c r="K5" t="n">
-        <v>32.62033985512386</v>
+        <v>29.44260597229004</v>
       </c>
       <c r="L5" t="n">
-        <v>403.4433334941343</v>
+        <v>402.1959838867188</v>
       </c>
       <c r="M5" t="n">
-        <v>347.1772678965466</v>
+        <v>348.1970825195312</v>
       </c>
       <c r="N5" t="n">
-        <v>319.8823794907339</v>
+        <v>318.8351745605469</v>
       </c>
       <c r="O5">
         <f>D5-E5</f>
@@ -644,47 +657,47 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IPSL-CM6A-LR</t>
+          <t>MRI-ESM2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.691160678863525</v>
+        <v>4.036277914891514</v>
       </c>
       <c r="C6" t="n">
-        <v>343.6947631835938</v>
+        <v>342.7713179570524</v>
       </c>
       <c r="D6" t="n">
-        <v>101.1413116455078</v>
+        <v>98.78611803032139</v>
       </c>
       <c r="E6" t="n">
-        <v>52.35886001586914</v>
+        <v>53.97546930750589</v>
       </c>
       <c r="F6" t="n">
-        <v>238.8623504638672</v>
+        <v>239.9489220118395</v>
       </c>
       <c r="G6" t="n">
-        <v>263.935791015625</v>
+        <v>264.3077792811944</v>
       </c>
       <c r="H6" t="n">
-        <v>189.9535064697266</v>
+        <v>192.4933452798664</v>
       </c>
       <c r="I6" t="n">
-        <v>249.1511383056641</v>
+        <v>245.8657745277478</v>
       </c>
       <c r="J6" t="n">
-        <v>23.22990036010742</v>
+        <v>26.85690586361529</v>
       </c>
       <c r="K6" t="n">
-        <v>29.44260597229004</v>
+        <v>32.62033985512386</v>
       </c>
       <c r="L6" t="n">
-        <v>402.1959838867188</v>
+        <v>403.4433334941343</v>
       </c>
       <c r="M6" t="n">
-        <v>348.1970825195312</v>
+        <v>347.1772678965466</v>
       </c>
       <c r="N6" t="n">
-        <v>318.8351745605469</v>
+        <v>319.8823794907339</v>
       </c>
       <c r="O6">
         <f>D6-E6</f>
@@ -1029,4 +1042,234 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="1200" orientation="portrait" paperSize="9" verticalDpi="1200"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="13.85546875"/>
+    <col customWidth="1" max="2" min="2" style="3" width="13.42578125"/>
+    <col customWidth="1" max="3" min="3" style="3" width="11.5703125"/>
+    <col customWidth="1" max="4" min="4" style="3" width="9.140625"/>
+    <col customWidth="1" max="5" min="5" style="3" width="20"/>
+    <col customWidth="1" max="6" min="6" width="16.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Good SWcs fit</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Insolation</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Albedo</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>r_liq</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>r_ice</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="E2" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>best for ensemble</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>GFDL-CM4</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>380</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>rlutcs under by 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CESM2-CAM6</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>378</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>rlutcs under by 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MRI-ESM2</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.036277054379609</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>342.7713118934579</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>98.78611701806761</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>53.97546924823823</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>239.9489180602529</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>264.3077785917636</v>
+      </c>
+      <c r="H6" t="n">
+        <v>192.4933453275627</v>
+      </c>
+      <c r="I6" t="n">
+        <v>245.8657797562242</v>
+      </c>
+      <c r="J6" t="n">
+        <v>26.85690608577296</v>
+      </c>
+      <c r="K6" t="n">
+        <v>32.62033959045065</v>
+      </c>
+      <c r="L6" t="n">
+        <v>403.4433355451918</v>
+      </c>
+      <c r="M6" t="n">
+        <v>347.1772706961048</v>
+      </c>
+      <c r="N6" t="n">
+        <v>319.8823832549311</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IPSL-CM6A-LR</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>382</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>rlutcs under by 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MRI-ESM2</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>380</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MIROC6</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>380</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="3" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RRTMG Climlab code working for model ensemble with alt, lat, time grid.
RRTMG Climlab code working for model ensemble with alt, lat, time grid.
</commit_message>
<xml_diff>
--- a/reduced_data/model_global_radiation_outputs_dt.xlsx
+++ b/reduced_data/model_global_radiation_outputs_dt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="34125" yWindow="-2565" windowWidth="21720" windowHeight="13830" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13830" windowWidth="21720" xWindow="34125" yWindow="-2565"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -89,38 +89,38 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -399,7 +399,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15.140625" customWidth="1" min="1" max="1"/>
+    <col customWidth="1" max="1" min="1" width="15.140625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1086,8 +1086,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="1200" verticalDpi="1200"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="1200" orientation="portrait" paperSize="9" verticalDpi="1200"/>
 </worksheet>
 </file>
 
@@ -1105,8 +1105,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="28.85546875" customWidth="1" min="1" max="1"/>
-    <col width="9.7109375" customWidth="1" min="2" max="2"/>
+    <col customWidth="1" max="1" min="1" width="28.85546875"/>
+    <col customWidth="1" max="2" min="2" width="9.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1151,50 +1151,29 @@
     <row r="2">
       <c r="A2" s="8" t="inlineStr">
         <is>
-          <t>CESM2-CAM6</t>
+          <t>Model Output</t>
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>4.433540775832256</v>
+        <v>50.17197</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>342.5167707485394</v>
+        <v>247.09817</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>98.5557595392647</v>
+        <v>262.99485</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>50.17197175769287</v>
+        <v>321.183526</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>239.0672615650613</v>
+        <v>98.55575</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>262.9948533577066</v>
-      </c>
-      <c r="H2" t="n">
-        <v>187.8756507608438</v>
-      </c>
-      <c r="I2" t="n">
-        <v>247.0981712702323</v>
-      </c>
-      <c r="J2" t="n">
-        <v>22.34518147134658</v>
-      </c>
-      <c r="K2" t="n">
-        <v>28.31099380915739</v>
-      </c>
-      <c r="L2" t="n">
-        <v>403.1150456921218</v>
-      </c>
-      <c r="M2" t="n">
-        <v>348.1831873899331</v>
-      </c>
-      <c r="N2" t="n">
-        <v>321.1835242648102</v>
-      </c>
-    </row>
-    <row r="3" ht="45" customHeight="1">
+        <v>239.06726</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
           <t>4-year time integrated with absorber and model insolation inputs</t>
@@ -1219,7 +1198,7 @@
         <v>244.12810098399</v>
       </c>
     </row>
-    <row r="4" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="4">
       <c r="A4" s="9" t="inlineStr">
         <is>
           <t>4-year time integrated model with insolation inputs and DEFAULT code absorber</t>
@@ -1244,7 +1223,7 @@
         <v>245.115512481746</v>
       </c>
     </row>
-    <row r="5" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="5">
       <c r="A5" s="9" t="inlineStr">
         <is>
           <t>4-year time integrated model with DEFAULT code absorber and insolation</t>
@@ -1270,15 +1249,52 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="n"/>
-      <c r="B6" s="11" t="n"/>
-      <c r="C6" s="11" t="n"/>
-      <c r="D6" s="11" t="n"/>
-      <c r="E6" s="11" t="n"/>
-      <c r="F6" s="11" t="n"/>
-      <c r="G6" s="11" t="n"/>
-    </row>
-    <row r="7" ht="45" customHeight="1">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>MRI-ESM2</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>4.036277054379609</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>342.7713118934579</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>98.78611701806761</v>
+      </c>
+      <c r="E6" s="11" t="n">
+        <v>53.97546924823823</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>239.9489180602529</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>264.3077785917636</v>
+      </c>
+      <c r="H6" t="n">
+        <v>192.4933453275627</v>
+      </c>
+      <c r="I6" t="n">
+        <v>245.8657797562242</v>
+      </c>
+      <c r="J6" t="n">
+        <v>26.85690608577296</v>
+      </c>
+      <c r="K6" t="n">
+        <v>32.62033959045065</v>
+      </c>
+      <c r="L6" t="n">
+        <v>403.4433355451918</v>
+      </c>
+      <c r="M6" t="n">
+        <v>347.1772706961048</v>
+      </c>
+      <c r="N6" t="n">
+        <v>319.8823832549311</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="45" r="7">
       <c r="A7" s="9" t="inlineStr">
         <is>
           <t>4-year mean model input with absorber and model insolation inputs</t>
@@ -1303,7 +1319,7 @@
         <v>244.052031294931</v>
       </c>
     </row>
-    <row r="8" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="8">
       <c r="A8" s="9" t="inlineStr">
         <is>
           <t>4-year mean model input with insolation inputs and DEFAULT code absorber</t>
@@ -1328,7 +1344,7 @@
         <v>245.073133210872</v>
       </c>
     </row>
-    <row r="9" ht="45" customHeight="1">
+    <row customHeight="1" ht="45" r="9">
       <c r="A9" s="9" t="inlineStr">
         <is>
           <t>4-year mean model input with DEFAULT code absorber and insolation</t>
@@ -1354,8 +1370,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="360" verticalDpi="360"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="360" orientation="portrait" paperSize="9" verticalDpi="360"/>
 </worksheet>
 </file>
 
@@ -1373,12 +1389,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.85546875" customWidth="1" min="1" max="1"/>
-    <col width="13.42578125" customWidth="1" style="3" min="2" max="2"/>
-    <col width="11.5703125" customWidth="1" style="3" min="3" max="3"/>
-    <col width="9.140625" customWidth="1" style="3" min="4" max="4"/>
-    <col width="20" customWidth="1" style="3" min="5" max="5"/>
-    <col width="16.42578125" customWidth="1" min="6" max="6"/>
+    <col customWidth="1" max="1" min="1" width="13.85546875"/>
+    <col customWidth="1" max="2" min="2" style="3" width="13.42578125"/>
+    <col customWidth="1" max="3" min="3" style="3" width="11.5703125"/>
+    <col customWidth="1" max="4" min="4" style="3" width="9.140625"/>
+    <col customWidth="1" max="5" min="5" style="3" width="20"/>
+    <col customWidth="1" max="6" min="6" width="16.42578125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1566,6 +1582,6 @@
       <c r="F9" s="3" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>